<commit_message>
Desenvolvido nova tela de adição de turmas
</commit_message>
<xml_diff>
--- a/WebContent/GatopolisManager.xlsx
+++ b/WebContent/GatopolisManager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="48620" yWindow="1560" windowWidth="20620" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Manager" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <t>SERIE</t>
   </si>
   <si>
-    <t>PERIODO (Manhã/Tarde)</t>
+    <t>PERIODO (MANHÃ/TARDE)</t>
   </si>
 </sst>
 </file>
@@ -432,16 +432,17 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="36" customHeight="1">

</xml_diff>

<commit_message>
Modelo relacional atualizado. Name adaptado para first_name e last_name
</commit_message>
<xml_diff>
--- a/WebContent/GatopolisManager.xlsx
+++ b/WebContent/GatopolisManager.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlapapalardo/Workspace/GatopolisManager/WebContent/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Manager" sheetId="1" r:id="rId1"/>
@@ -19,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>NOME COMPLETO DO ALUNO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>SEXO (Menino/Menina)</t>
   </si>
@@ -40,6 +42,12 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>NOME  DO ALUNO</t>
+  </si>
+  <si>
+    <t>SOBRENOME DO ALUNO</t>
   </si>
 </sst>
 </file>
@@ -109,6 +117,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -434,52 +447,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="44.5" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="1" max="2" width="44.5" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="36" customHeight="1">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="F2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="E2" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>